<commit_message>
added fuzzy matching for all files
</commit_message>
<xml_diff>
--- a/chris/Data/liquidated_debt_certificates_DE.xlsx
+++ b/chris/Data/liquidated_debt_certificates_DE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisliao/Google Drive/Non-Academic Work/Research/Sargent/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisliao/Google Drive/Non-Academic Work/Research/Sargent/SPEOC-pt-1/chris/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDB2CA0-F1A2-6149-BB8E-1A284B276F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D204B9E-5FCE-A64C-BC0F-8B89192DF0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="500" windowWidth="14320" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1759,22 +1759,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1792,6 +1789,21 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1800,18 +1812,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2165,7 +2165,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2384,25 +2384,25 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="39" t="s">
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="40" t="s">
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="41" t="s">
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="41"/>
+      <c r="N10" s="42"/>
       <c r="O10" s="33"/>
       <c r="P10" s="35"/>
       <c r="Q10" s="3"/>
@@ -2424,52 +2424,52 @@
       <c r="AL10" s="37"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="49" t="s">
+      <c r="I11" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="51" t="s">
+      <c r="K11" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="42" t="s">
+      <c r="L11" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="52" t="s">
+      <c r="M11" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="55" t="s">
+      <c r="N11" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="53" t="s">
+      <c r="O11" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="P11" s="54" t="s">
+      <c r="P11" s="40" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="26"/>
@@ -2492,22 +2492,22 @@
       <c r="AL11" s="25"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="54"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="40"/>
       <c r="Q12" s="26"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
@@ -30861,22 +30861,22 @@
     <sortCondition ref="C13:C637"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="P11:P12"/>
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="L11:L12"/>

</xml_diff>